<commit_message>
changement pour affichage du fichier compétence plus rapide
</commit_message>
<xml_diff>
--- a/documents/competences.xlsx
+++ b/documents/competences.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2">
   <fileVersion appName="Calc"/>
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
@@ -37,7 +37,7 @@
     <t xml:space="preserve">N° candidat : </t>
   </si>
   <si>
-    <t xml:space="preserve">Centre de formation :Lycée Félix Le Dantec</t>
+    <t xml:space="preserve">Centre de formation : Lycée Félix Le Dantec</t>
   </si>
   <si>
     <t xml:space="preserve">Option :</t>
@@ -153,7 +153,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="13">
+  <fonts count="12">
     <font>
       <sz val="10"/>
       <color theme="1"/>
@@ -231,12 +231,6 @@
       <name val="Arial"/>
       <family val="0"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="0"/>
     </font>
     <font>
       <sz val="8"/>
@@ -549,7 +543,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="36">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -654,27 +648,15 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -686,11 +668,11 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="19" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="19" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -702,7 +684,7 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -786,37 +768,37 @@
         <a:srgbClr val="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:srgbClr val="ffffff"/>
+        <a:srgbClr val="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="000000"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="ffffff"/>
+        <a:srgbClr val="FFFFFF"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="4f81bd"/>
+        <a:srgbClr val="4F81BD"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="c0504d"/>
+        <a:srgbClr val="C0504D"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="9bbb59"/>
+        <a:srgbClr val="9BBB59"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="8064a2"/>
+        <a:srgbClr val="8064A2"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4bacc6"/>
+        <a:srgbClr val="4BACC6"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="f79646"/>
+        <a:srgbClr val="F79646"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0000ff"/>
+        <a:srgbClr val="0000FF"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="0000ff"/>
+        <a:srgbClr val="0000FF"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Sheets">
@@ -957,8 +939,8 @@
   </sheetPr>
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1210,14 +1192,6 @@
       <c r="Z9" s="4"/>
     </row>
     <row r="10" customFormat="false" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0"/>
-      <c r="B10" s="0"/>
-      <c r="C10" s="0"/>
-      <c r="D10" s="0"/>
-      <c r="E10" s="0"/>
-      <c r="F10" s="0"/>
-      <c r="G10" s="0"/>
-      <c r="H10" s="0"/>
       <c r="I10" s="4"/>
       <c r="J10" s="4"/>
       <c r="K10" s="4"/>
@@ -1238,14 +1212,6 @@
       <c r="Z10" s="4"/>
     </row>
     <row r="11" customFormat="false" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0"/>
-      <c r="B11" s="0"/>
-      <c r="C11" s="0"/>
-      <c r="D11" s="0"/>
-      <c r="E11" s="0"/>
-      <c r="F11" s="0"/>
-      <c r="G11" s="0"/>
-      <c r="H11" s="0"/>
       <c r="I11" s="4"/>
       <c r="J11" s="4"/>
       <c r="K11" s="4"/>
@@ -1464,26 +1430,26 @@
       <c r="Z18" s="4"/>
     </row>
     <row r="19" customFormat="false" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="26" t="s">
+      <c r="A19" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="B19" s="27" t="s">
+      <c r="B19" s="26" t="s">
         <v>31</v>
       </c>
-      <c r="C19" s="28" t="s">
+      <c r="C19" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="D19" s="29" t="s">
+      <c r="D19" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="E19" s="29" t="s">
+      <c r="E19" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="F19" s="29" t="s">
+      <c r="F19" s="20" t="s">
         <v>26</v>
       </c>
       <c r="G19" s="17"/>
-      <c r="H19" s="28" t="s">
+      <c r="H19" s="17" t="s">
         <v>26</v>
       </c>
       <c r="I19" s="4"/>
@@ -1508,12 +1474,12 @@
     <row r="20" customFormat="false" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="21"/>
       <c r="B20" s="22"/>
-      <c r="C20" s="30"/>
-      <c r="D20" s="30"/>
-      <c r="E20" s="30"/>
-      <c r="F20" s="30"/>
-      <c r="G20" s="30"/>
-      <c r="H20" s="31"/>
+      <c r="C20" s="27"/>
+      <c r="D20" s="27"/>
+      <c r="E20" s="27"/>
+      <c r="F20" s="27"/>
+      <c r="G20" s="27"/>
+      <c r="H20" s="28"/>
       <c r="I20" s="4"/>
       <c r="J20" s="4"/>
       <c r="K20" s="4"/>
@@ -1536,12 +1502,12 @@
     <row r="21" customFormat="false" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="21"/>
       <c r="B21" s="22"/>
-      <c r="C21" s="30"/>
-      <c r="D21" s="30"/>
-      <c r="E21" s="30"/>
-      <c r="F21" s="30"/>
-      <c r="G21" s="30"/>
-      <c r="H21" s="31"/>
+      <c r="C21" s="27"/>
+      <c r="D21" s="27"/>
+      <c r="E21" s="27"/>
+      <c r="F21" s="27"/>
+      <c r="G21" s="27"/>
+      <c r="H21" s="28"/>
       <c r="I21" s="4"/>
       <c r="J21" s="4"/>
       <c r="K21" s="4"/>
@@ -1564,12 +1530,12 @@
     <row r="22" customFormat="false" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="21"/>
       <c r="B22" s="22"/>
-      <c r="C22" s="30"/>
-      <c r="D22" s="30"/>
-      <c r="E22" s="30"/>
-      <c r="F22" s="30"/>
-      <c r="G22" s="30"/>
-      <c r="H22" s="31"/>
+      <c r="C22" s="27"/>
+      <c r="D22" s="27"/>
+      <c r="E22" s="27"/>
+      <c r="F22" s="27"/>
+      <c r="G22" s="27"/>
+      <c r="H22" s="28"/>
       <c r="I22" s="4"/>
       <c r="J22" s="4"/>
       <c r="K22" s="4"/>
@@ -1592,12 +1558,12 @@
     <row r="23" customFormat="false" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="21"/>
       <c r="B23" s="23"/>
-      <c r="C23" s="30"/>
-      <c r="D23" s="30"/>
-      <c r="E23" s="30"/>
-      <c r="F23" s="30"/>
-      <c r="G23" s="30"/>
-      <c r="H23" s="31"/>
+      <c r="C23" s="27"/>
+      <c r="D23" s="27"/>
+      <c r="E23" s="27"/>
+      <c r="F23" s="27"/>
+      <c r="G23" s="27"/>
+      <c r="H23" s="28"/>
       <c r="I23" s="4"/>
       <c r="J23" s="4"/>
       <c r="K23" s="4"/>
@@ -1620,12 +1586,12 @@
     <row r="24" customFormat="false" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="21"/>
       <c r="B24" s="23"/>
-      <c r="C24" s="30"/>
-      <c r="D24" s="30"/>
-      <c r="E24" s="30"/>
-      <c r="F24" s="30"/>
-      <c r="G24" s="30"/>
-      <c r="H24" s="31"/>
+      <c r="C24" s="27"/>
+      <c r="D24" s="27"/>
+      <c r="E24" s="27"/>
+      <c r="F24" s="27"/>
+      <c r="G24" s="27"/>
+      <c r="H24" s="28"/>
       <c r="I24" s="4"/>
       <c r="J24" s="4"/>
       <c r="K24" s="4"/>
@@ -1648,12 +1614,12 @@
     <row r="25" customFormat="false" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="21"/>
       <c r="B25" s="23"/>
-      <c r="C25" s="30"/>
-      <c r="D25" s="30"/>
-      <c r="E25" s="30"/>
-      <c r="F25" s="30"/>
-      <c r="G25" s="30"/>
-      <c r="H25" s="31"/>
+      <c r="C25" s="27"/>
+      <c r="D25" s="27"/>
+      <c r="E25" s="27"/>
+      <c r="F25" s="27"/>
+      <c r="G25" s="27"/>
+      <c r="H25" s="28"/>
       <c r="I25" s="4"/>
       <c r="J25" s="4"/>
       <c r="K25" s="4"/>
@@ -1676,12 +1642,12 @@
     <row r="26" customFormat="false" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="21"/>
       <c r="B26" s="23"/>
-      <c r="C26" s="30"/>
-      <c r="D26" s="30"/>
-      <c r="E26" s="30"/>
-      <c r="F26" s="30"/>
-      <c r="G26" s="30"/>
-      <c r="H26" s="31"/>
+      <c r="C26" s="27"/>
+      <c r="D26" s="27"/>
+      <c r="E26" s="27"/>
+      <c r="F26" s="27"/>
+      <c r="G26" s="27"/>
+      <c r="H26" s="28"/>
       <c r="I26" s="4"/>
       <c r="J26" s="4"/>
       <c r="K26" s="4"/>
@@ -1732,26 +1698,26 @@
       <c r="Z27" s="4"/>
     </row>
     <row r="28" customFormat="false" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A28" s="26" t="s">
+      <c r="A28" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="B28" s="27" t="s">
+      <c r="B28" s="26" t="s">
         <v>34</v>
       </c>
-      <c r="C28" s="29" t="s">
+      <c r="C28" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="D28" s="29" t="s">
+      <c r="D28" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="E28" s="29" t="s">
+      <c r="E28" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="F28" s="29" t="s">
+      <c r="F28" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="G28" s="30"/>
-      <c r="H28" s="31"/>
+      <c r="G28" s="27"/>
+      <c r="H28" s="28"/>
       <c r="I28" s="4"/>
       <c r="J28" s="4"/>
       <c r="K28" s="4"/>
@@ -1774,12 +1740,12 @@
     <row r="29" customFormat="false" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="21"/>
       <c r="B29" s="23"/>
-      <c r="C29" s="30"/>
-      <c r="D29" s="30"/>
-      <c r="E29" s="30"/>
-      <c r="F29" s="30"/>
-      <c r="G29" s="30"/>
-      <c r="H29" s="31"/>
+      <c r="C29" s="27"/>
+      <c r="D29" s="27"/>
+      <c r="E29" s="27"/>
+      <c r="F29" s="27"/>
+      <c r="G29" s="27"/>
+      <c r="H29" s="28"/>
       <c r="I29" s="4"/>
       <c r="J29" s="4"/>
       <c r="K29" s="4"/>
@@ -1802,12 +1768,12 @@
     <row r="30" customFormat="false" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="21"/>
       <c r="B30" s="23"/>
-      <c r="C30" s="30"/>
-      <c r="D30" s="30"/>
-      <c r="E30" s="30"/>
-      <c r="F30" s="30"/>
-      <c r="G30" s="30"/>
-      <c r="H30" s="31"/>
+      <c r="C30" s="27"/>
+      <c r="D30" s="27"/>
+      <c r="E30" s="27"/>
+      <c r="F30" s="27"/>
+      <c r="G30" s="27"/>
+      <c r="H30" s="28"/>
       <c r="I30" s="4"/>
       <c r="J30" s="4"/>
       <c r="K30" s="4"/>
@@ -1830,12 +1796,12 @@
     <row r="31" customFormat="false" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="21"/>
       <c r="B31" s="23"/>
-      <c r="C31" s="30"/>
-      <c r="D31" s="30"/>
-      <c r="E31" s="30"/>
-      <c r="F31" s="30"/>
-      <c r="G31" s="30"/>
-      <c r="H31" s="31"/>
+      <c r="C31" s="27"/>
+      <c r="D31" s="27"/>
+      <c r="E31" s="27"/>
+      <c r="F31" s="27"/>
+      <c r="G31" s="27"/>
+      <c r="H31" s="28"/>
       <c r="I31" s="4"/>
       <c r="J31" s="4"/>
       <c r="K31" s="4"/>
@@ -1858,12 +1824,12 @@
     <row r="32" customFormat="false" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="21"/>
       <c r="B32" s="23"/>
-      <c r="C32" s="30"/>
-      <c r="D32" s="30"/>
-      <c r="E32" s="30"/>
-      <c r="F32" s="30"/>
-      <c r="G32" s="30"/>
-      <c r="H32" s="31"/>
+      <c r="C32" s="27"/>
+      <c r="D32" s="27"/>
+      <c r="E32" s="27"/>
+      <c r="F32" s="27"/>
+      <c r="G32" s="27"/>
+      <c r="H32" s="28"/>
       <c r="I32" s="4"/>
       <c r="J32" s="4"/>
       <c r="K32" s="4"/>
@@ -1886,12 +1852,12 @@
     <row r="33" customFormat="false" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="21"/>
       <c r="B33" s="23"/>
-      <c r="C33" s="30"/>
-      <c r="D33" s="30"/>
-      <c r="E33" s="30"/>
-      <c r="F33" s="30"/>
-      <c r="G33" s="30"/>
-      <c r="H33" s="31"/>
+      <c r="C33" s="27"/>
+      <c r="D33" s="27"/>
+      <c r="E33" s="27"/>
+      <c r="F33" s="27"/>
+      <c r="G33" s="27"/>
+      <c r="H33" s="28"/>
       <c r="I33" s="4"/>
       <c r="J33" s="4"/>
       <c r="K33" s="4"/>
@@ -1914,12 +1880,12 @@
     <row r="34" customFormat="false" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="21"/>
       <c r="B34" s="23"/>
-      <c r="C34" s="30"/>
-      <c r="D34" s="30"/>
-      <c r="E34" s="30"/>
-      <c r="F34" s="30"/>
-      <c r="G34" s="30"/>
-      <c r="H34" s="31"/>
+      <c r="C34" s="27"/>
+      <c r="D34" s="27"/>
+      <c r="E34" s="27"/>
+      <c r="F34" s="27"/>
+      <c r="G34" s="27"/>
+      <c r="H34" s="28"/>
       <c r="I34" s="4"/>
       <c r="J34" s="4"/>
       <c r="K34" s="4"/>
@@ -1940,14 +1906,14 @@
       <c r="Z34" s="4"/>
     </row>
     <row r="35" customFormat="false" ht="39.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A35" s="32"/>
-      <c r="B35" s="33"/>
-      <c r="C35" s="34"/>
-      <c r="D35" s="34"/>
-      <c r="E35" s="34"/>
-      <c r="F35" s="34"/>
-      <c r="G35" s="34"/>
-      <c r="H35" s="35"/>
+      <c r="A35" s="29"/>
+      <c r="B35" s="30"/>
+      <c r="C35" s="31"/>
+      <c r="D35" s="31"/>
+      <c r="E35" s="31"/>
+      <c r="F35" s="31"/>
+      <c r="G35" s="31"/>
+      <c r="H35" s="32"/>
       <c r="I35" s="4"/>
       <c r="J35" s="4"/>
       <c r="K35" s="4"/>
@@ -1968,14 +1934,14 @@
       <c r="Z35" s="4"/>
     </row>
     <row r="36" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A36" s="36"/>
-      <c r="B36" s="37"/>
-      <c r="C36" s="38"/>
-      <c r="D36" s="38"/>
-      <c r="E36" s="38"/>
-      <c r="F36" s="38"/>
-      <c r="G36" s="38"/>
-      <c r="H36" s="38"/>
+      <c r="A36" s="33"/>
+      <c r="B36" s="34"/>
+      <c r="C36" s="35"/>
+      <c r="D36" s="35"/>
+      <c r="E36" s="35"/>
+      <c r="F36" s="35"/>
+      <c r="G36" s="35"/>
+      <c r="H36" s="35"/>
       <c r="I36" s="4"/>
       <c r="J36" s="4"/>
       <c r="K36" s="4"/>

</xml_diff>